<commit_message>
adding zaken to Arch.adl
</commit_message>
<xml_diff>
--- a/Blik/Wetsartikelen.xlsx
+++ b/Blik/Wetsartikelen.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="195" yWindow="75" windowWidth="15300" windowHeight="7950" activeTab="1"/>
+    <workbookView xWindow="195" yWindow="135" windowWidth="15300" windowHeight="7890" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Wetsartikelen" sheetId="3" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="416">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="526">
   <si>
     <t>Wet handhaving consumentenbescherming</t>
   </si>
@@ -1263,6 +1263,336 @@
   </si>
   <si>
     <t>Aantal</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0005537/</t>
+  </si>
+  <si>
+    <t>BWBR0005537</t>
+  </si>
+  <si>
+    <t>Algemene Wet Bestuursrecht</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0020586/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0002075/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019795/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0013798/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0018823/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0017347/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035217/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0005758/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0009828/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0005489/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035091/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032386/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0022233/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0010009/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032657/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0008223/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0029746/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0033323/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0015167/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0018370/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0007216/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0009675/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0031405/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0024291/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0036129/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032262/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0033809/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019074/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0036080/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0018989/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0011673/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032518/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0004284/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032626/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0028123/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0007049/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019229/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0036106/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019227/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0007087/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0011594/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0002600/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0013864/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0036431/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0034301/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0033925/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0020572/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032516/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0029884/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0036837/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0030962/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035074/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035950/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0017176/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0017341/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0031531/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0036430/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0017587/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0031503/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0023007/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0022543/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0007923/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0007248/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0005835/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0013946/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0028149/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0020740/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032462/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032146/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019575/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0022545/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0034311/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035248/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0014538/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0020800/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0033362/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032975/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0024915/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0034303/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0034876/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035708/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0018397/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0012616/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0022420/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0022975/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0005528/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032771/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0032751/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0012617/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0037073/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019235/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035180/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0006003/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0015945/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0006736/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0024539/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0030288/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0035516/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0010600/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0027118/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0024023/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0034872/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0020507/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019442/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0019228/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0010434/</t>
+  </si>
+  <si>
+    <t>http://wetten.overheid.nl/BWBR0021907/</t>
   </si>
 </sst>
 </file>
@@ -4455,12 +4785,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D109"/>
+  <dimension ref="A1:D110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
+    <col min="2" max="2" width="56.5703125" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="3"/>
   </cols>
   <sheetData>
@@ -4502,9 +4836,8 @@
       <c r="C3" s="3">
         <v>61</v>
       </c>
-      <c r="D3" t="str">
-        <f>"http://wetten.overheid.nl/"&amp;A3&amp;"/"</f>
-        <v>http://wetten.overheid.nl/BWBR0020586/</v>
+      <c r="D3" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -4517,9 +4850,8 @@
       <c r="C4" s="3">
         <v>18</v>
       </c>
-      <c r="D4" t="str">
-        <f t="shared" ref="D4:D67" si="0">"http://wetten.overheid.nl/"&amp;A4&amp;"/"</f>
-        <v>http://wetten.overheid.nl/BWBR0002075/</v>
+      <c r="D4" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -4532,9 +4864,8 @@
       <c r="C5" s="3">
         <v>14</v>
       </c>
-      <c r="D5" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0019795/</v>
+      <c r="D5" t="s">
+        <v>421</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4547,9 +4878,8 @@
       <c r="C6" s="3">
         <v>47</v>
       </c>
-      <c r="D6" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0013798/</v>
+      <c r="D6" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -4562,9 +4892,8 @@
       <c r="C7" s="3">
         <v>20</v>
       </c>
-      <c r="D7" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0018823/</v>
+      <c r="D7" t="s">
+        <v>423</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -4577,9 +4906,8 @@
       <c r="C8" s="3">
         <v>12</v>
       </c>
-      <c r="D8" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0017347/</v>
+      <c r="D8" t="s">
+        <v>424</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -4592,9 +4920,8 @@
       <c r="C9" s="3">
         <v>196</v>
       </c>
-      <c r="D9" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0035217/</v>
+      <c r="D9" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4607,9 +4934,8 @@
       <c r="C10" s="3">
         <v>26</v>
       </c>
-      <c r="D10" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0005758/</v>
+      <c r="D10" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -4622,9 +4948,8 @@
       <c r="C11" s="3">
         <v>21</v>
       </c>
-      <c r="D11" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0009828/</v>
+      <c r="D11" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -4637,9 +4962,8 @@
       <c r="C12" s="3">
         <v>18</v>
       </c>
-      <c r="D12" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0005489/</v>
+      <c r="D12" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -4652,9 +4976,8 @@
       <c r="C13" s="3">
         <v>54</v>
       </c>
-      <c r="D13" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0035091/</v>
+      <c r="D13" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4667,9 +4990,8 @@
       <c r="C14" s="3">
         <v>112</v>
       </c>
-      <c r="D14" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0032386/</v>
+      <c r="D14" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -4682,9 +5004,8 @@
       <c r="C15" s="3">
         <v>21</v>
       </c>
-      <c r="D15" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0022233/</v>
+      <c r="D15" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -4697,9 +5018,8 @@
       <c r="C16" s="3">
         <v>4</v>
       </c>
-      <c r="D16" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0010009/</v>
+      <c r="D16" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -4712,9 +5032,8 @@
       <c r="C17" s="3">
         <v>6</v>
       </c>
-      <c r="D17" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0032657/</v>
+      <c r="D17" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -4727,9 +5046,8 @@
       <c r="C18" s="3">
         <v>34</v>
       </c>
-      <c r="D18" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0008223/</v>
+      <c r="D18" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -4742,9 +5060,8 @@
       <c r="C19" s="3">
         <v>12</v>
       </c>
-      <c r="D19" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0029746/</v>
+      <c r="D19" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -4757,9 +5074,8 @@
       <c r="C20" s="3">
         <v>33</v>
       </c>
-      <c r="D20" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0033323/</v>
+      <c r="D20" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -4772,9 +5088,8 @@
       <c r="C21" s="3">
         <v>20</v>
       </c>
-      <c r="D21" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0015167/</v>
+      <c r="D21" t="s">
+        <v>437</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
@@ -4787,9 +5102,8 @@
       <c r="C22" s="3">
         <v>15</v>
       </c>
-      <c r="D22" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0018370/</v>
+      <c r="D22" t="s">
+        <v>438</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4802,9 +5116,8 @@
       <c r="C23" s="3">
         <v>11</v>
       </c>
-      <c r="D23" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0007216/</v>
+      <c r="D23" t="s">
+        <v>439</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -4817,9 +5130,8 @@
       <c r="C24" s="3">
         <v>17</v>
       </c>
-      <c r="D24" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0009675/</v>
+      <c r="D24" t="s">
+        <v>440</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -4832,9 +5144,8 @@
       <c r="C25" s="3">
         <v>13</v>
       </c>
-      <c r="D25" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0031405/</v>
+      <c r="D25" t="s">
+        <v>441</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -4847,9 +5158,8 @@
       <c r="C26" s="3">
         <v>178</v>
       </c>
-      <c r="D26" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0024291/</v>
+      <c r="D26" t="s">
+        <v>442</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -4862,9 +5172,8 @@
       <c r="C27" s="3">
         <v>9</v>
       </c>
-      <c r="D27" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0036129/</v>
+      <c r="D27" t="s">
+        <v>443</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4877,9 +5186,8 @@
       <c r="C28" s="3">
         <v>5</v>
       </c>
-      <c r="D28" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0032262/</v>
+      <c r="D28" t="s">
+        <v>444</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -4892,9 +5200,8 @@
       <c r="C29" s="3">
         <v>4</v>
       </c>
-      <c r="D29" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0033809/</v>
+      <c r="D29" t="s">
+        <v>445</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4907,9 +5214,8 @@
       <c r="C30" s="3">
         <v>6</v>
       </c>
-      <c r="D30" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0019074/</v>
+      <c r="D30" t="s">
+        <v>446</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
@@ -4922,9 +5228,8 @@
       <c r="C31" s="3">
         <v>25</v>
       </c>
-      <c r="D31" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0036080/</v>
+      <c r="D31" t="s">
+        <v>447</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4937,9 +5242,8 @@
       <c r="C32" s="3">
         <v>193</v>
       </c>
-      <c r="D32" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0018989/</v>
+      <c r="D32" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
@@ -4952,9 +5256,8 @@
       <c r="C33" s="3">
         <v>24</v>
       </c>
-      <c r="D33" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0011673/</v>
+      <c r="D33" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4967,9 +5270,8 @@
       <c r="C34" s="3">
         <v>7</v>
       </c>
-      <c r="D34" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0032518/</v>
+      <c r="D34" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
@@ -4982,9 +5284,8 @@
       <c r="C35" s="3">
         <v>20</v>
       </c>
-      <c r="D35" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0004284/</v>
+      <c r="D35" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4997,9 +5298,8 @@
       <c r="C36" s="3">
         <v>169</v>
       </c>
-      <c r="D36" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0032626/</v>
+      <c r="D36" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
@@ -5012,9 +5312,8 @@
       <c r="C37" s="3">
         <v>49</v>
       </c>
-      <c r="D37" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0028123/</v>
+      <c r="D37" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
@@ -5027,9 +5326,8 @@
       <c r="C38" s="3">
         <v>208</v>
       </c>
-      <c r="D38" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0007049/</v>
+      <c r="D38" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
@@ -5042,9 +5340,8 @@
       <c r="C39" s="3">
         <v>7</v>
       </c>
-      <c r="D39" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0019229/</v>
+      <c r="D39" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
@@ -5057,9 +5354,8 @@
       <c r="C40" s="3">
         <v>18</v>
       </c>
-      <c r="D40" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0036106/</v>
+      <c r="D40" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -5072,9 +5368,8 @@
       <c r="C41" s="3">
         <v>7</v>
       </c>
-      <c r="D41" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0019227/</v>
+      <c r="D41" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -5087,9 +5382,8 @@
       <c r="C42" s="3">
         <v>17</v>
       </c>
-      <c r="D42" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0007087/</v>
+      <c r="D42" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
@@ -5102,9 +5396,8 @@
       <c r="C43" s="3">
         <v>2</v>
       </c>
-      <c r="D43" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0011594/</v>
+      <c r="D43" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -5117,9 +5410,8 @@
       <c r="C44" s="3">
         <v>2</v>
       </c>
-      <c r="D44" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0002600/</v>
+      <c r="D44" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
@@ -5132,9 +5424,8 @@
       <c r="C45" s="3">
         <v>3</v>
       </c>
-      <c r="D45" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0013864/</v>
+      <c r="D45" t="s">
+        <v>461</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -5147,9 +5438,8 @@
       <c r="C46" s="3">
         <v>3</v>
       </c>
-      <c r="D46" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0036431/</v>
+      <c r="D46" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
@@ -5162,9 +5452,8 @@
       <c r="C47" s="3">
         <v>12</v>
       </c>
-      <c r="D47" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0034301/</v>
+      <c r="D47" t="s">
+        <v>463</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
@@ -5177,9 +5466,8 @@
       <c r="C48" s="3">
         <v>5</v>
       </c>
-      <c r="D48" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0033925/</v>
+      <c r="D48" t="s">
+        <v>464</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -5192,9 +5480,8 @@
       <c r="C49" s="3">
         <v>3</v>
       </c>
-      <c r="D49" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0020572/</v>
+      <c r="D49" t="s">
+        <v>465</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
@@ -5207,9 +5494,8 @@
       <c r="C50" s="3">
         <v>4</v>
       </c>
-      <c r="D50" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0032516/</v>
+      <c r="D50" t="s">
+        <v>466</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
@@ -5222,9 +5508,8 @@
       <c r="C51" s="3">
         <v>3</v>
       </c>
-      <c r="D51" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0029884/</v>
+      <c r="D51" t="s">
+        <v>467</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
@@ -5237,9 +5522,8 @@
       <c r="C52" s="3">
         <v>4</v>
       </c>
-      <c r="D52" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0036837/</v>
+      <c r="D52" t="s">
+        <v>468</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
@@ -5252,9 +5536,8 @@
       <c r="C53" s="3">
         <v>10</v>
       </c>
-      <c r="D53" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0030962/</v>
+      <c r="D53" t="s">
+        <v>469</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
@@ -5267,9 +5550,8 @@
       <c r="C54" s="3">
         <v>4</v>
       </c>
-      <c r="D54" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0035074/</v>
+      <c r="D54" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
@@ -5282,9 +5564,8 @@
       <c r="C55" s="3">
         <v>8</v>
       </c>
-      <c r="D55" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0035950/</v>
+      <c r="D55" t="s">
+        <v>471</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
@@ -5297,9 +5578,8 @@
       <c r="C56" s="3">
         <v>2</v>
       </c>
-      <c r="D56" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0017176/</v>
+      <c r="D56" t="s">
+        <v>472</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
@@ -5312,9 +5592,8 @@
       <c r="C57" s="3">
         <v>2</v>
       </c>
-      <c r="D57" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0017341/</v>
+      <c r="D57" t="s">
+        <v>473</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
@@ -5327,9 +5606,8 @@
       <c r="C58" s="3">
         <v>2</v>
       </c>
-      <c r="D58" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0031531/</v>
+      <c r="D58" t="s">
+        <v>474</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
@@ -5342,9 +5620,8 @@
       <c r="C59" s="3">
         <v>3</v>
       </c>
-      <c r="D59" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0036430/</v>
+      <c r="D59" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
@@ -5357,9 +5634,8 @@
       <c r="C60" s="3">
         <v>7</v>
       </c>
-      <c r="D60" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0017587/</v>
+      <c r="D60" t="s">
+        <v>476</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
@@ -5372,9 +5648,8 @@
       <c r="C61" s="3">
         <v>6</v>
       </c>
-      <c r="D61" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0031503/</v>
+      <c r="D61" t="s">
+        <v>477</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
@@ -5387,9 +5662,8 @@
       <c r="C62" s="3">
         <v>10</v>
       </c>
-      <c r="D62" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0023007/</v>
+      <c r="D62" t="s">
+        <v>478</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
@@ -5402,9 +5676,8 @@
       <c r="C63" s="3">
         <v>24</v>
       </c>
-      <c r="D63" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0022543/</v>
+      <c r="D63" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
@@ -5417,9 +5690,8 @@
       <c r="C64" s="3">
         <v>24</v>
       </c>
-      <c r="D64" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0007923/</v>
+      <c r="D64" t="s">
+        <v>480</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
@@ -5432,9 +5704,8 @@
       <c r="C65" s="3">
         <v>2</v>
       </c>
-      <c r="D65" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0007248/</v>
+      <c r="D65" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
@@ -5447,9 +5718,8 @@
       <c r="C66" s="3">
         <v>5</v>
       </c>
-      <c r="D66" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0005835/</v>
+      <c r="D66" t="s">
+        <v>482</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
@@ -5462,9 +5732,8 @@
       <c r="C67" s="3">
         <v>33</v>
       </c>
-      <c r="D67" t="str">
-        <f t="shared" si="0"/>
-        <v>http://wetten.overheid.nl/BWBR0013946/</v>
+      <c r="D67" t="s">
+        <v>483</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
@@ -5477,9 +5746,8 @@
       <c r="C68" s="3">
         <v>8</v>
       </c>
-      <c r="D68" t="str">
-        <f t="shared" ref="D68:D109" si="1">"http://wetten.overheid.nl/"&amp;A68&amp;"/"</f>
-        <v>http://wetten.overheid.nl/BWBR0028149/</v>
+      <c r="D68" t="s">
+        <v>484</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
@@ -5492,9 +5760,8 @@
       <c r="C69" s="3">
         <v>28</v>
       </c>
-      <c r="D69" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0020740/</v>
+      <c r="D69" t="s">
+        <v>485</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
@@ -5507,9 +5774,8 @@
       <c r="C70" s="3">
         <v>95</v>
       </c>
-      <c r="D70" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0032462/</v>
+      <c r="D70" t="s">
+        <v>486</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
@@ -5522,9 +5788,8 @@
       <c r="C71" s="3">
         <v>7</v>
       </c>
-      <c r="D71" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0032146/</v>
+      <c r="D71" t="s">
+        <v>487</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
@@ -5537,9 +5802,8 @@
       <c r="C72" s="3">
         <v>37</v>
       </c>
-      <c r="D72" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0019575/</v>
+      <c r="D72" t="s">
+        <v>488</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
@@ -5552,9 +5816,8 @@
       <c r="C73" s="3">
         <v>53</v>
       </c>
-      <c r="D73" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0022545/</v>
+      <c r="D73" t="s">
+        <v>489</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
@@ -5567,9 +5830,8 @@
       <c r="C74" s="3">
         <v>12</v>
       </c>
-      <c r="D74" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0034311/</v>
+      <c r="D74" t="s">
+        <v>490</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
@@ -5582,9 +5844,8 @@
       <c r="C75" s="3">
         <v>63</v>
       </c>
-      <c r="D75" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0035248/</v>
+      <c r="D75" t="s">
+        <v>491</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
@@ -5597,9 +5858,8 @@
       <c r="C76" s="3">
         <v>127</v>
       </c>
-      <c r="D76" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0014538/</v>
+      <c r="D76" t="s">
+        <v>492</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
@@ -5612,9 +5872,8 @@
       <c r="C77" s="3">
         <v>44</v>
       </c>
-      <c r="D77" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0020800/</v>
+      <c r="D77" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
@@ -5627,9 +5886,8 @@
       <c r="C78" s="3">
         <v>12</v>
       </c>
-      <c r="D78" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0033362/</v>
+      <c r="D78" t="s">
+        <v>494</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
@@ -5642,9 +5900,8 @@
       <c r="C79" s="3">
         <v>35</v>
       </c>
-      <c r="D79" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0032975/</v>
+      <c r="D79" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.25">
@@ -5657,9 +5914,8 @@
       <c r="C80" s="3">
         <v>132</v>
       </c>
-      <c r="D80" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0024915/</v>
+      <c r="D80" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.25">
@@ -5672,9 +5928,8 @@
       <c r="C81" s="3">
         <v>8</v>
       </c>
-      <c r="D81" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0034303/</v>
+      <c r="D81" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
@@ -5687,9 +5942,8 @@
       <c r="C82" s="3">
         <v>33</v>
       </c>
-      <c r="D82" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0034876/</v>
+      <c r="D82" t="s">
+        <v>498</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
@@ -5702,9 +5956,8 @@
       <c r="C83" s="3">
         <v>33</v>
       </c>
-      <c r="D83" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0035708/</v>
+      <c r="D83" t="s">
+        <v>499</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
@@ -5717,9 +5970,8 @@
       <c r="C84" s="3">
         <v>201</v>
       </c>
-      <c r="D84" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0018397/</v>
+      <c r="D84" t="s">
+        <v>500</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
@@ -5732,9 +5984,8 @@
       <c r="C85" s="3">
         <v>31</v>
       </c>
-      <c r="D85" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0012616/</v>
+      <c r="D85" t="s">
+        <v>501</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
@@ -5747,9 +5998,8 @@
       <c r="C86" s="3">
         <v>58</v>
       </c>
-      <c r="D86" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0022420/</v>
+      <c r="D86" t="s">
+        <v>502</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
@@ -5762,9 +6012,8 @@
       <c r="C87" s="3">
         <v>46</v>
       </c>
-      <c r="D87" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0022975/</v>
+      <c r="D87" t="s">
+        <v>503</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
@@ -5777,9 +6026,8 @@
       <c r="C88" s="3">
         <v>2</v>
       </c>
-      <c r="D88" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0005528/</v>
+      <c r="D88" t="s">
+        <v>504</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
@@ -5792,9 +6040,8 @@
       <c r="C89" s="3">
         <v>6</v>
       </c>
-      <c r="D89" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0032771/</v>
+      <c r="D89" t="s">
+        <v>505</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
@@ -5807,9 +6054,8 @@
       <c r="C90" s="3">
         <v>6</v>
       </c>
-      <c r="D90" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0032751/</v>
+      <c r="D90" t="s">
+        <v>506</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
@@ -5822,9 +6068,8 @@
       <c r="C91" s="3">
         <v>32</v>
       </c>
-      <c r="D91" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0012617/</v>
+      <c r="D91" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
@@ -5837,9 +6082,8 @@
       <c r="C92" s="3">
         <v>3</v>
       </c>
-      <c r="D92" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0037073/</v>
+      <c r="D92" t="s">
+        <v>508</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.25">
@@ -5852,9 +6096,8 @@
       <c r="C93" s="3">
         <v>70</v>
       </c>
-      <c r="D93" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0019235/</v>
+      <c r="D93" t="s">
+        <v>509</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
@@ -5867,9 +6110,8 @@
       <c r="C94" s="3">
         <v>25</v>
       </c>
-      <c r="D94" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0035180/</v>
+      <c r="D94" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
@@ -5882,9 +6124,8 @@
       <c r="C95" s="3">
         <v>12</v>
       </c>
-      <c r="D95" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0006003/</v>
+      <c r="D95" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
@@ -5897,9 +6138,8 @@
       <c r="C96" s="3">
         <v>9</v>
       </c>
-      <c r="D96" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0015945/</v>
+      <c r="D96" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.25">
@@ -5912,9 +6152,8 @@
       <c r="C97" s="3">
         <v>47</v>
       </c>
-      <c r="D97" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0006736/</v>
+      <c r="D97" t="s">
+        <v>513</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.25">
@@ -5927,9 +6166,8 @@
       <c r="C98" s="3">
         <v>103</v>
       </c>
-      <c r="D98" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0024539/</v>
+      <c r="D98" t="s">
+        <v>514</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.25">
@@ -5942,9 +6180,8 @@
       <c r="C99" s="3">
         <v>151</v>
       </c>
-      <c r="D99" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0030288/</v>
+      <c r="D99" t="s">
+        <v>515</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.25">
@@ -5957,9 +6194,8 @@
       <c r="C100" s="3">
         <v>5</v>
       </c>
-      <c r="D100" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0035516/</v>
+      <c r="D100" t="s">
+        <v>516</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.25">
@@ -5972,9 +6208,8 @@
       <c r="C101" s="3">
         <v>11</v>
       </c>
-      <c r="D101" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0010600/</v>
+      <c r="D101" t="s">
+        <v>517</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.25">
@@ -5987,9 +6222,8 @@
       <c r="C102" s="3">
         <v>7</v>
       </c>
-      <c r="D102" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0027118/</v>
+      <c r="D102" t="s">
+        <v>518</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.25">
@@ -6002,9 +6236,8 @@
       <c r="C103" s="3">
         <v>5</v>
       </c>
-      <c r="D103" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0024023/</v>
+      <c r="D103" t="s">
+        <v>519</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.25">
@@ -6017,9 +6250,8 @@
       <c r="C104" s="3">
         <v>9</v>
       </c>
-      <c r="D104" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0034872/</v>
+      <c r="D104" t="s">
+        <v>520</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.25">
@@ -6032,9 +6264,8 @@
       <c r="C105" s="3">
         <v>5</v>
       </c>
-      <c r="D105" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0020507/</v>
+      <c r="D105" t="s">
+        <v>521</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.25">
@@ -6047,9 +6278,8 @@
       <c r="C106" s="3">
         <v>6</v>
       </c>
-      <c r="D106" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0019442/</v>
+      <c r="D106" t="s">
+        <v>522</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.25">
@@ -6062,9 +6292,8 @@
       <c r="C107" s="3">
         <v>4</v>
       </c>
-      <c r="D107" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0019228/</v>
+      <c r="D107" t="s">
+        <v>523</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.25">
@@ -6077,9 +6306,8 @@
       <c r="C108" s="3">
         <v>9</v>
       </c>
-      <c r="D108" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0010434/</v>
+      <c r="D108" t="s">
+        <v>524</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.25">
@@ -6092,12 +6320,28 @@
       <c r="C109" s="3">
         <v>11</v>
       </c>
-      <c r="D109" t="str">
-        <f t="shared" si="1"/>
-        <v>http://wetten.overheid.nl/BWBR0021907/</v>
+      <c r="D109" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>417</v>
+      </c>
+      <c r="B110" t="s">
+        <v>418</v>
+      </c>
+      <c r="C110" s="3">
+        <v>518</v>
+      </c>
+      <c r="D110" t="s">
+        <v>416</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D110" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>